<commit_message>
remove different HLA containing the sample full length sequences
</commit_message>
<xml_diff>
--- a/HLA.xlsx
+++ b/HLA.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/vy/Desktop/GS/TCR-datasets/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{63144745-9B92-2046-A599-90AC53DB3707}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B6B2219B-6E23-2348-AC9C-056809151D80}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-23000" yWindow="-21600" windowWidth="38400" windowHeight="21600" activeTab="2" xr2:uid="{C1B0ED54-1291-CB41-9802-DB7407159840}"/>
+    <workbookView xWindow="35840" yWindow="3120" windowWidth="30240" windowHeight="17180" activeTab="2" xr2:uid="{C1B0ED54-1291-CB41-9802-DB7407159840}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="728" uniqueCount="394">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="695" uniqueCount="384">
   <si>
     <t>A*02</t>
   </si>
@@ -873,9 +873,6 @@
     <t>MRVTAPRTVLLLLWGAVALTETWAGSHSMRYFYTAMSRPGRGEPRFIAVGYVDDTQFVRFDSDAASPRTEPRAPWIEQEGPEYWDRNTQIFKTNTQTYRENLRIALRYYNQSEAGSHTWQTMYGCDVGPDGRLLRGHNQYAYDGKDYIALNEDLSSWTAADTAAQITQRKWEAAREAEQLRAYLEGLCVEWLRRHLENGKETLQRADPPKTHVTHHPVSDHEATLRCWALGFYPAEITLTWQRDGEDQTQDTELVETRPAGDRTFQKWAAVVVPSGEEQRYTCHVQHEGLPKPLTLRWEPSSQSTIPIVGIVAGLAVLAVVVIGAVVATVMCRRKSSGGKGGSYSQAASSDSAQGSDVSLTA</t>
   </si>
   <si>
-    <t>https://www.ebi.ac.uk/ipd/imgt/hla/alleles/allele/?accession=HLA11724</t>
-  </si>
-  <si>
     <t>https://www.ebi.ac.uk/ipd/imgt/hla/alleles/allele/?accession=HLA00090</t>
   </si>
   <si>
@@ -900,9 +897,6 @@
     <t>MILNKALLLGALALTTVMSPCGGEDIVADHVASCGVNLYQFYGPSGQFTHEFDGDEQFYVDLEKKETAWRWPEFSKFGGFDPQGALRNMAVAKHNLNIMIKRYNSTAATNEVPEVTVFSKSPVTLGQPNTLICLVDNIFPPVVNITWLSNGHAVTEGVSETSFLSKSDHSFFKISYLTFLPSADEIYDCKVEHWGLDQPLLKHWEPEIPAPMSELTETVVCALGLSVGLVGIVVGTVFIIQGLRSVGASRHQGPL</t>
   </si>
   <si>
-    <t>https://www.ebi.ac.uk/ipd/imgt/hla/alleles/allele/?accession=HLA13212</t>
-  </si>
-  <si>
     <t>https://www.ebi.ac.uk/ipd/imgt/hla/alleles/allele/?accession=HLA06657</t>
   </si>
   <si>
@@ -921,9 +915,6 @@
     <t>MAISGVPVLGFFIIAVLMSAQESWAIKEEHVIIQAEFYLNPDQSGEFMFDFDGDEIFHVDMAKKETVWRLEEFGRFASFEAQGALANIAVDKANLEIMTKRSNYTPITNVPPEVTVLTNSPVELREPNVLICFIDKFTPPVVNVTWLRNGKPVTTGVSETVFLPREDHLFRKFHYLPFLPSTEDVYDCRVEHWGLDEPLLKHWEFDAPSPLPETTENVVCALGLTVGLVGIIIGTIFIIKGLRKSNAAERRGPL</t>
   </si>
   <si>
-    <t>https://www.ebi.ac.uk/ipd/imgt/hla/alleles/allele/?accession=HLA06468</t>
-  </si>
-  <si>
     <t>https://www.ebi.ac.uk/ipd/imgt/hla/alleles/allele/?accession=HLA00446</t>
   </si>
   <si>
@@ -960,9 +951,6 @@
     <t>MVDGTLLLLLSEALALTQTWAGSHSLKYFHTSVSRPGRGEPRFISVGYVDDTQFVRFDNDAASPRMVPRAPWMEQEGSEYWDRETRSARDTAQIFRVNLRTLRGYYNQSEAGSHTLQWMHGCELGPDRRFLRGYEQFAYDGKDYLTLNEDLRSWTAVDTAAQISEQKSNDASEAEHQRAYLEDTCVEWLHKYLEKGKETLLHLEPPKTHVTHHPISDHEATLRCWALGFYPAEITLTWQQDGEGHTQDTELVETRPAGDGTFQKWAAVVVPSGEEQRYTCHVQHEGLPEPVTLRWKPASQPTIPIVGIIAGLVLLGSVVSGAVVAAVIWRKKSSGGKGGSYSKAEWSDSAQGSESHSL</t>
   </si>
   <si>
-    <t>https://www.ebi.ac.uk/ipd/imgt/hla/alleles/allele/?accession=HLA12720</t>
-  </si>
-  <si>
     <t>https://www.ebi.ac.uk/ipd/imgt/hla/alleles/allele/?accession=HLA00602</t>
   </si>
   <si>
@@ -975,21 +963,12 @@
     <t>MAVMAPRTLVLLLSGALALTQTWAGSHSMRYFFTSVSRPGRGEPRFIAVGYVDDTQFVRFDSDAASQRMEPRAPWIEQEGPEYWDGETRKVKAHSQTHRVDLGTLRGYYNQSEAGSHTVQRMYGCDVGSDWRFLRGYHQYAYDGKDYIALKEDLRSWTAADMAAQTTKHKWEAAHVAEQLRAYLEGTCVEWLRRYLENGKETLQRTDAPKTHMTHHAVSDHEATLRCWALSFYPAEITLTWQRDGEDQTQDTELVETRPAGDGTFQKWAAVVVPSGQEQRYTCHVQHEGLPKPLTLRWEPSSQPTIPIVGIIAGLVLFGAVITGAVVAAVMWRRKSS</t>
   </si>
   <si>
-    <t>https://www.ebi.ac.uk/ipd/imgt/hla/alleles/allele/?accession=HLA14075</t>
-  </si>
-  <si>
     <t>https://www.ebi.ac.uk/ipd/imgt/hla/alleles/allele/?accession=HLA06618</t>
   </si>
   <si>
     <t>MILNKALMLGALALTTVMSPCGGEDIVADHVASYGVNLYQSYGPSGQYTHEFDGDEQFYVDLGRKETVWCLPVLRQFRFDPQFALTNIAVLKHNLNSLIKRSNSTAATNEVPEVTVFSKSPVTLGQPNILICLVDNIFPPVVNITWLSNGHSVTEGVSETSFLSKSDHSFFKISYLTLLPSAEESYDCKVEHWGLDKPLLKHWEPEIPAPMSELTETVVCALGLSVGLVGIVVGTVFIIRGLRSVGASRHQGPL</t>
   </si>
   <si>
-    <t>https://www.ebi.ac.uk/ipd/imgt/hla/alleles/allele/?accession=HLA13357</t>
-  </si>
-  <si>
-    <t>https://www.ebi.ac.uk/ipd/imgt/hla/alleles/allele/?accession=HLA13791</t>
-  </si>
-  <si>
     <t>MILNKALMLGALALTTVMSPCGGEDIVADHVASYGVNLYQSYGPSGQFTHEFDGDEEFYVDLERKETVWKLPLFHRLRFDPQFALTNIAVLKHNLNILIKRSNSTAATNEVPEVTVFSKSPVTLGQPNTLICLVDNIFPPVVNITWLSNGHSVTEGVSETSFLSKSDHSFFKISYLTFLPSADEIYDCKVEHWGLDEPLLKHWEPEIPAPMSELTETVVCALGLSVGLVGIVVGTVLIIRGLRSVGASRHQGPL</t>
   </si>
   <si>
@@ -1008,9 +987,6 @@
     <t>MRPEDRMFHIRAVILRALSLAFLLSLRGAGAIKADHVSTYAAFVQTHRPTGEFMFEFDEDEMFYVDLDKKETVWHLEEFGQAFSFEAQGGLANIAILNNNLNTLIQRSNHTQATNDPPEVTVFPKEPVELGQPNTLICHIDKFFPPVLNVTWLCNGELVTEGVAESLFLPRTDYSFHKFHYLTFVPSAEDFYDCRVEHWGLDQPLLKHWEAQEPIQMPETTETVLCALGLVLGLVGIIVGTVLIIKSLRSGHDPRAQGTL</t>
   </si>
   <si>
-    <t>https://www.ebi.ac.uk/ipd/imgt/hla/alleles/allele/?accession=HLA05114</t>
-  </si>
-  <si>
     <t>https://www.ebi.ac.uk/ipd/imgt/hla/alleles/allele/?accession=HLA00433</t>
   </si>
   <si>
@@ -1065,16 +1041,10 @@
     <t>MRVTAPRTVLLLLWGAVALTETWAGSHSMRYFYTAMSRPGRGEPRFIAVGYVDDTQFVRFDSDAASPRMAPRAPWIEQEGPEYWDGETRNMKASAQTYRENLRIALRYYNQSEAGSHIIQVMYGCDVGPDGRLLRGHDQSAYDGKDYIALNEDLSSWTAADTAAQIIQRKWEAARVAEQLRAYLEGLCVEWLRRYLENGKETLQRADPPKTHVTHHPISDHEATLRCWALGFYPAEITLTWQRDGEDQTQDTELVETRPAGDRTFQKWAAVVVPSGEEQRYTCHVQHEGLPKPLTLRWEPSSQSTVPIVGIVAGLAVLAVVVIGAVVAAVMCRRKSSGGKGGSYSQAACSDSAQGSDVSLTA</t>
   </si>
   <si>
-    <t>https://www.ebi.ac.uk/ipd/imgt/hla/alleles/allele/?accession=HLA02432</t>
-  </si>
-  <si>
     <t>https://www.ebi.ac.uk/ipd/imgt/hla/alleles/allele/?accession=HLA08433</t>
   </si>
   <si>
     <t>MILNKALLLGALALTTVMSPCGGEDIVADHVASCGVNLYQFYGPSGQYTHEFDGDEQFYVDLERKETAWRWPEFSKFGGFDPQGALRNMAVAKHNLNIMIKRYNSTAATNEVPEVTVFSKSPVTLGQPNTLICLVDNIFPPVVNITWLSNGQSVTEGVSETSFLSKSDHSFFKISYLTFLPSADEIYDCKVEHWGLDQPLLKHWEPEILAPMSELTETVVCALGLSVGLMGIVVGTVFIIQGLRSVGASRHQGPL</t>
-  </si>
-  <si>
-    <t>https://www.ebi.ac.uk/ipd/imgt/hla/alleles/allele/?accession=HLA05239</t>
   </si>
   <si>
     <t>https://www.ebi.ac.uk/ipd/imgt/hla/alleles/allele/?accession=HLA00619</t>
@@ -1573,7 +1543,7 @@
   <dimension ref="A1:F29"/>
   <sheetViews>
     <sheetView zoomScale="156" workbookViewId="0">
-      <selection activeCell="A23" sqref="A23"/>
+      <selection activeCell="D19" sqref="D19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2146,8 +2116,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{97B4ACF3-4489-5643-B74E-93909852E9EA}">
   <dimension ref="A1:C181"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+    <sheetView topLeftCell="A56" workbookViewId="0">
+      <selection activeCell="B75" sqref="B75"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2163,7 +2133,7 @@
         <v>250</v>
       </c>
       <c r="C1" t="s">
-        <v>393</v>
+        <v>383</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.2">
@@ -2440,7 +2410,7 @@
         <v>17</v>
       </c>
       <c r="B36" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="37" spans="1:3" x14ac:dyDescent="0.2">
@@ -2541,7 +2511,7 @@
         <v>112</v>
       </c>
       <c r="B49" t="s">
-        <v>112</v>
+        <v>24</v>
       </c>
     </row>
     <row r="50" spans="1:2" x14ac:dyDescent="0.2">
@@ -2613,7 +2583,7 @@
         <v>121</v>
       </c>
       <c r="B58" t="s">
-        <v>121</v>
+        <v>82</v>
       </c>
     </row>
     <row r="59" spans="1:2" x14ac:dyDescent="0.2">
@@ -2645,7 +2615,7 @@
         <v>125</v>
       </c>
       <c r="B62" t="s">
-        <v>125</v>
+        <v>97</v>
       </c>
     </row>
     <row r="63" spans="1:2" x14ac:dyDescent="0.2">
@@ -2701,7 +2671,7 @@
         <v>132</v>
       </c>
       <c r="B69" t="s">
-        <v>132</v>
+        <v>126</v>
       </c>
     </row>
     <row r="70" spans="1:2" x14ac:dyDescent="0.2">
@@ -2725,7 +2695,7 @@
         <v>135</v>
       </c>
       <c r="B72" t="s">
-        <v>135</v>
+        <v>74</v>
       </c>
     </row>
     <row r="73" spans="1:2" x14ac:dyDescent="0.2">
@@ -2741,7 +2711,7 @@
         <v>137</v>
       </c>
       <c r="B74" t="s">
-        <v>137</v>
+        <v>25</v>
       </c>
     </row>
     <row r="75" spans="1:2" x14ac:dyDescent="0.2">
@@ -2749,7 +2719,7 @@
         <v>138</v>
       </c>
       <c r="B75" t="s">
-        <v>138</v>
+        <v>23</v>
       </c>
     </row>
     <row r="76" spans="1:2" x14ac:dyDescent="0.2">
@@ -2810,7 +2780,7 @@
         <v>146</v>
       </c>
       <c r="B83" t="s">
-        <v>146</v>
+        <v>19</v>
       </c>
     </row>
     <row r="84" spans="1:3" x14ac:dyDescent="0.2">
@@ -2996,7 +2966,7 @@
         <v>170</v>
       </c>
       <c r="B107" t="s">
-        <v>170</v>
+        <v>133</v>
       </c>
     </row>
     <row r="108" spans="1:2" x14ac:dyDescent="0.2">
@@ -3020,7 +2990,7 @@
         <v>173</v>
       </c>
       <c r="B110" t="s">
-        <v>173</v>
+        <v>20</v>
       </c>
     </row>
     <row r="111" spans="1:2" x14ac:dyDescent="0.2">
@@ -3544,10 +3514,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B4608C81-BCF1-0849-B7B2-1CC7E0824005}">
-  <dimension ref="A1:D135"/>
+  <dimension ref="A1:D124"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C136" sqref="C136"/>
+    <sheetView tabSelected="1" topLeftCell="A37" workbookViewId="0">
+      <selection activeCell="N48" sqref="N48"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -3835,103 +3805,94 @@
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
-        <v>17</v>
+        <v>101</v>
       </c>
       <c r="B25" t="s">
-        <v>33</v>
+        <v>270</v>
       </c>
       <c r="C25">
-        <v>365</v>
+        <v>362</v>
       </c>
       <c r="D25" t="s">
-        <v>36</v>
+        <v>271</v>
       </c>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
-        <v>101</v>
-      </c>
-      <c r="B26" t="s">
-        <v>270</v>
-      </c>
-      <c r="C26">
-        <v>362</v>
-      </c>
-      <c r="D26" t="s">
-        <v>271</v>
+        <v>241</v>
       </c>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
-        <v>241</v>
+        <v>104</v>
       </c>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
-        <v>104</v>
+        <v>106</v>
+      </c>
+      <c r="B28" t="s">
+        <v>273</v>
+      </c>
+      <c r="C28">
+        <v>365</v>
+      </c>
+      <c r="D28" t="s">
+        <v>272</v>
       </c>
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
       <c r="B29" t="s">
-        <v>273</v>
+        <v>274</v>
       </c>
       <c r="C29">
-        <v>365</v>
+        <v>362</v>
       </c>
       <c r="D29" t="s">
-        <v>272</v>
+        <v>275</v>
       </c>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
-        <v>107</v>
-      </c>
-      <c r="B30" t="s">
-        <v>274</v>
-      </c>
-      <c r="C30">
-        <v>362</v>
-      </c>
-      <c r="D30" t="s">
-        <v>275</v>
+        <v>108</v>
       </c>
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
-        <v>108</v>
+        <v>109</v>
+      </c>
+      <c r="B31" t="s">
+        <v>277</v>
+      </c>
+      <c r="C31">
+        <v>362</v>
+      </c>
+      <c r="D31" t="s">
+        <v>276</v>
       </c>
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
-        <v>109</v>
-      </c>
-      <c r="B32" t="s">
-        <v>277</v>
-      </c>
-      <c r="C32">
-        <v>362</v>
-      </c>
-      <c r="D32" t="s">
-        <v>276</v>
+        <v>110</v>
       </c>
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
-        <v>110</v>
+        <v>113</v>
       </c>
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
-        <v>112</v>
+        <v>114</v>
       </c>
       <c r="B34" t="s">
-        <v>66</v>
+        <v>279</v>
       </c>
       <c r="C34">
-        <v>362</v>
+        <v>365</v>
       </c>
       <c r="D34" t="s">
         <v>278</v>
@@ -3939,29 +3900,29 @@
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
-        <v>113</v>
+        <v>115</v>
+      </c>
+      <c r="B35" t="s">
+        <v>280</v>
+      </c>
+      <c r="C35">
+        <v>362</v>
+      </c>
+      <c r="D35" t="s">
+        <v>281</v>
       </c>
     </row>
     <row r="36" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
-        <v>114</v>
-      </c>
-      <c r="B36" t="s">
-        <v>280</v>
-      </c>
-      <c r="C36">
-        <v>365</v>
-      </c>
-      <c r="D36" t="s">
-        <v>279</v>
+        <v>116</v>
       </c>
     </row>
     <row r="37" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
-        <v>115</v>
+        <v>117</v>
       </c>
       <c r="B37" t="s">
-        <v>281</v>
+        <v>283</v>
       </c>
       <c r="C37">
         <v>362</v>
@@ -3972,1029 +3933,884 @@
     </row>
     <row r="38" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
-        <v>116</v>
+        <v>118</v>
+      </c>
+      <c r="B38" t="s">
+        <v>285</v>
+      </c>
+      <c r="C38">
+        <v>255</v>
+      </c>
+      <c r="D38" t="s">
+        <v>284</v>
       </c>
     </row>
     <row r="39" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
-        <v>117</v>
-      </c>
-      <c r="B39" t="s">
-        <v>284</v>
-      </c>
-      <c r="C39">
-        <v>362</v>
-      </c>
-      <c r="D39" t="s">
-        <v>283</v>
+        <v>119</v>
       </c>
     </row>
     <row r="40" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
-        <v>118</v>
-      </c>
-      <c r="B40" t="s">
-        <v>286</v>
-      </c>
-      <c r="C40">
-        <v>255</v>
-      </c>
-      <c r="D40" t="s">
-        <v>285</v>
+        <v>120</v>
       </c>
     </row>
     <row r="41" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A41" t="s">
-        <v>119</v>
+        <v>122</v>
+      </c>
+      <c r="B41" t="s">
+        <v>287</v>
+      </c>
+      <c r="C41">
+        <v>298</v>
+      </c>
+      <c r="D41" t="s">
+        <v>286</v>
       </c>
     </row>
     <row r="42" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A42" t="s">
-        <v>120</v>
+        <v>123</v>
+      </c>
+      <c r="B42" t="s">
+        <v>289</v>
+      </c>
+      <c r="C42">
+        <v>298</v>
+      </c>
+      <c r="D42" t="s">
+        <v>288</v>
       </c>
     </row>
     <row r="43" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A43" t="s">
-        <v>121</v>
+        <v>124</v>
       </c>
       <c r="B43" t="s">
-        <v>261</v>
+        <v>291</v>
       </c>
       <c r="C43">
-        <v>362</v>
+        <v>254</v>
       </c>
       <c r="D43" t="s">
-        <v>287</v>
+        <v>290</v>
       </c>
     </row>
     <row r="44" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A44" t="s">
-        <v>122</v>
+        <v>126</v>
       </c>
       <c r="B44" t="s">
-        <v>289</v>
+        <v>293</v>
       </c>
       <c r="C44">
-        <v>298</v>
+        <v>366</v>
       </c>
       <c r="D44" t="s">
-        <v>288</v>
+        <v>292</v>
       </c>
     </row>
     <row r="45" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A45" t="s">
-        <v>123</v>
+        <v>127</v>
       </c>
       <c r="B45" t="s">
-        <v>291</v>
+        <v>295</v>
       </c>
       <c r="C45">
-        <v>298</v>
+        <v>362</v>
       </c>
       <c r="D45" t="s">
-        <v>290</v>
+        <v>294</v>
       </c>
     </row>
     <row r="46" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A46" t="s">
-        <v>124</v>
+        <v>128</v>
       </c>
       <c r="B46" t="s">
-        <v>293</v>
+        <v>297</v>
       </c>
       <c r="C46">
-        <v>254</v>
+        <v>337</v>
       </c>
       <c r="D46" t="s">
-        <v>292</v>
+        <v>296</v>
       </c>
     </row>
     <row r="47" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A47" t="s">
-        <v>125</v>
+        <v>129</v>
       </c>
       <c r="B47" t="s">
-        <v>269</v>
+        <v>298</v>
       </c>
       <c r="C47">
-        <v>254</v>
+        <v>362</v>
       </c>
       <c r="D47" t="s">
-        <v>294</v>
+        <v>299</v>
       </c>
     </row>
     <row r="48" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A48" t="s">
-        <v>126</v>
+        <v>130</v>
       </c>
       <c r="B48" t="s">
-        <v>296</v>
+        <v>301</v>
       </c>
       <c r="C48">
-        <v>366</v>
+        <v>255</v>
       </c>
       <c r="D48" t="s">
-        <v>295</v>
+        <v>300</v>
       </c>
     </row>
     <row r="49" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A49" t="s">
-        <v>127</v>
+        <v>131</v>
       </c>
       <c r="B49" t="s">
-        <v>298</v>
+        <v>303</v>
       </c>
       <c r="C49">
-        <v>362</v>
+        <v>358</v>
       </c>
       <c r="D49" t="s">
-        <v>297</v>
+        <v>302</v>
       </c>
     </row>
     <row r="50" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A50" t="s">
-        <v>128</v>
+        <v>133</v>
       </c>
       <c r="B50" t="s">
-        <v>300</v>
+        <v>305</v>
       </c>
       <c r="C50">
-        <v>337</v>
+        <v>255</v>
       </c>
       <c r="D50" t="s">
-        <v>299</v>
+        <v>304</v>
       </c>
     </row>
     <row r="51" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A51" t="s">
-        <v>129</v>
+        <v>134</v>
       </c>
       <c r="B51" t="s">
-        <v>301</v>
+        <v>307</v>
       </c>
       <c r="C51">
-        <v>362</v>
+        <v>337</v>
       </c>
       <c r="D51" t="s">
-        <v>302</v>
+        <v>306</v>
       </c>
     </row>
     <row r="52" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A52" t="s">
-        <v>130</v>
+        <v>136</v>
       </c>
       <c r="B52" t="s">
-        <v>304</v>
+        <v>309</v>
       </c>
       <c r="C52">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="D52" t="s">
-        <v>303</v>
+        <v>308</v>
       </c>
     </row>
     <row r="53" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A53" t="s">
-        <v>131</v>
+        <v>139</v>
       </c>
       <c r="B53" t="s">
-        <v>306</v>
+        <v>310</v>
       </c>
       <c r="C53">
-        <v>358</v>
+        <v>254</v>
       </c>
       <c r="D53" t="s">
-        <v>305</v>
+        <v>311</v>
       </c>
     </row>
     <row r="54" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A54" t="s">
-        <v>132</v>
-      </c>
-      <c r="B54" t="s">
-        <v>296</v>
-      </c>
-      <c r="C54">
-        <v>366</v>
-      </c>
-      <c r="D54" t="s">
-        <v>307</v>
+        <v>140</v>
       </c>
     </row>
     <row r="55" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A55" t="s">
-        <v>133</v>
+        <v>141</v>
       </c>
       <c r="B55" t="s">
-        <v>309</v>
+        <v>313</v>
       </c>
       <c r="C55">
-        <v>255</v>
+        <v>365</v>
       </c>
       <c r="D55" t="s">
-        <v>308</v>
+        <v>312</v>
       </c>
     </row>
     <row r="56" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A56" t="s">
-        <v>134</v>
-      </c>
-      <c r="B56" t="s">
-        <v>311</v>
-      </c>
-      <c r="C56">
-        <v>337</v>
-      </c>
-      <c r="D56" t="s">
-        <v>310</v>
+        <v>142</v>
       </c>
     </row>
     <row r="57" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A57" t="s">
-        <v>135</v>
+        <v>143</v>
       </c>
       <c r="B57" t="s">
-        <v>40</v>
+        <v>315</v>
       </c>
       <c r="C57">
-        <v>365</v>
+        <v>260</v>
       </c>
       <c r="D57" t="s">
-        <v>312</v>
+        <v>314</v>
       </c>
     </row>
     <row r="58" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A58" t="s">
-        <v>136</v>
-      </c>
-      <c r="B58" t="s">
-        <v>314</v>
-      </c>
-      <c r="C58">
-        <v>254</v>
-      </c>
-      <c r="D58" t="s">
-        <v>313</v>
+        <v>144</v>
       </c>
     </row>
     <row r="59" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A59" t="s">
-        <v>137</v>
+        <v>246</v>
       </c>
       <c r="B59" t="s">
-        <v>70</v>
+        <v>317</v>
       </c>
       <c r="C59">
-        <v>362</v>
+        <v>366</v>
       </c>
       <c r="D59" t="s">
-        <v>315</v>
+        <v>316</v>
       </c>
     </row>
     <row r="60" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A60" t="s">
-        <v>138</v>
-      </c>
-      <c r="B60" t="s">
-        <v>61</v>
-      </c>
-      <c r="C60">
-        <v>362</v>
-      </c>
-      <c r="D60" t="s">
-        <v>316</v>
+        <v>149</v>
       </c>
     </row>
     <row r="61" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A61" t="s">
-        <v>139</v>
-      </c>
-      <c r="B61" t="s">
-        <v>317</v>
-      </c>
-      <c r="C61">
-        <v>254</v>
-      </c>
-      <c r="D61" t="s">
-        <v>318</v>
+        <v>150</v>
       </c>
     </row>
     <row r="62" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A62" t="s">
-        <v>140</v>
+        <v>151</v>
       </c>
     </row>
     <row r="63" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A63" t="s">
-        <v>141</v>
-      </c>
-      <c r="B63" t="s">
-        <v>320</v>
-      </c>
-      <c r="C63">
-        <v>365</v>
-      </c>
-      <c r="D63" t="s">
-        <v>319</v>
+        <v>152</v>
       </c>
     </row>
     <row r="64" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A64" t="s">
-        <v>142</v>
+        <v>153</v>
       </c>
     </row>
     <row r="65" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A65" t="s">
-        <v>143</v>
+        <v>154</v>
       </c>
       <c r="B65" t="s">
-        <v>322</v>
+        <v>319</v>
       </c>
       <c r="C65">
-        <v>260</v>
+        <v>362</v>
       </c>
       <c r="D65" t="s">
-        <v>321</v>
+        <v>318</v>
       </c>
     </row>
     <row r="66" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A66" t="s">
-        <v>144</v>
+        <v>155</v>
       </c>
     </row>
     <row r="67" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A67" t="s">
-        <v>146</v>
-      </c>
-      <c r="B67" t="s">
-        <v>44</v>
-      </c>
-      <c r="C67">
-        <v>365</v>
-      </c>
-      <c r="D67" t="s">
-        <v>323</v>
+        <v>156</v>
       </c>
     </row>
     <row r="68" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A68" t="s">
-        <v>246</v>
-      </c>
-      <c r="B68" t="s">
-        <v>325</v>
-      </c>
-      <c r="C68">
-        <v>366</v>
-      </c>
-      <c r="D68" t="s">
-        <v>324</v>
+        <v>157</v>
       </c>
     </row>
     <row r="69" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A69" t="s">
-        <v>149</v>
+        <v>159</v>
+      </c>
+      <c r="B69" t="s">
+        <v>321</v>
+      </c>
+      <c r="C69">
+        <v>337</v>
+      </c>
+      <c r="D69" t="s">
+        <v>320</v>
       </c>
     </row>
     <row r="70" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A70" t="s">
-        <v>150</v>
+        <v>160</v>
+      </c>
+      <c r="B70" t="s">
+        <v>323</v>
+      </c>
+      <c r="C70">
+        <v>366</v>
+      </c>
+      <c r="D70" t="s">
+        <v>322</v>
       </c>
     </row>
     <row r="71" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A71" t="s">
-        <v>151</v>
+        <v>162</v>
+      </c>
+      <c r="B71" t="s">
+        <v>325</v>
+      </c>
+      <c r="C71">
+        <v>340</v>
+      </c>
+      <c r="D71" t="s">
+        <v>324</v>
       </c>
     </row>
     <row r="72" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A72" t="s">
-        <v>152</v>
+        <v>163</v>
+      </c>
+      <c r="B72" t="s">
+        <v>326</v>
+      </c>
+      <c r="C72">
+        <v>365</v>
+      </c>
+      <c r="D72" t="s">
+        <v>327</v>
       </c>
     </row>
     <row r="73" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A73" t="s">
-        <v>153</v>
+        <v>165</v>
+      </c>
+      <c r="B73" t="s">
+        <v>329</v>
+      </c>
+      <c r="C73">
+        <v>365</v>
+      </c>
+      <c r="D73" t="s">
+        <v>328</v>
       </c>
     </row>
     <row r="74" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A74" t="s">
-        <v>154</v>
+        <v>166</v>
       </c>
       <c r="B74" t="s">
-        <v>327</v>
+        <v>331</v>
       </c>
       <c r="C74">
-        <v>362</v>
+        <v>254</v>
       </c>
       <c r="D74" t="s">
-        <v>326</v>
+        <v>330</v>
       </c>
     </row>
     <row r="75" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A75" t="s">
-        <v>155</v>
+        <v>167</v>
       </c>
     </row>
     <row r="76" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A76" t="s">
-        <v>156</v>
+        <v>168</v>
       </c>
     </row>
     <row r="77" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A77" t="s">
-        <v>157</v>
+        <v>169</v>
+      </c>
+      <c r="B77" t="s">
+        <v>333</v>
+      </c>
+      <c r="C77">
+        <v>362</v>
+      </c>
+      <c r="D77" t="s">
+        <v>332</v>
       </c>
     </row>
     <row r="78" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A78" t="s">
-        <v>159</v>
+        <v>171</v>
       </c>
       <c r="B78" t="s">
-        <v>329</v>
+        <v>335</v>
       </c>
       <c r="C78">
-        <v>337</v>
+        <v>255</v>
       </c>
       <c r="D78" t="s">
-        <v>328</v>
+        <v>334</v>
       </c>
     </row>
     <row r="79" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A79" t="s">
-        <v>160</v>
-      </c>
-      <c r="B79" t="s">
-        <v>331</v>
-      </c>
-      <c r="C79">
-        <v>366</v>
-      </c>
-      <c r="D79" t="s">
-        <v>330</v>
+        <v>172</v>
       </c>
     </row>
     <row r="80" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A80" t="s">
-        <v>162</v>
+        <v>174</v>
       </c>
       <c r="B80" t="s">
-        <v>333</v>
+        <v>337</v>
       </c>
       <c r="C80">
-        <v>340</v>
+        <v>254</v>
       </c>
       <c r="D80" t="s">
-        <v>332</v>
+        <v>336</v>
       </c>
     </row>
     <row r="81" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A81" t="s">
-        <v>163</v>
+        <v>175</v>
       </c>
       <c r="B81" t="s">
-        <v>334</v>
+        <v>339</v>
       </c>
       <c r="C81">
-        <v>365</v>
+        <v>260</v>
       </c>
       <c r="D81" t="s">
-        <v>335</v>
+        <v>338</v>
       </c>
     </row>
     <row r="82" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A82" t="s">
-        <v>165</v>
+        <v>247</v>
       </c>
       <c r="B82" t="s">
-        <v>337</v>
+        <v>341</v>
       </c>
       <c r="C82">
-        <v>365</v>
+        <v>366</v>
       </c>
       <c r="D82" t="s">
-        <v>336</v>
+        <v>340</v>
       </c>
     </row>
     <row r="83" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A83" t="s">
-        <v>166</v>
-      </c>
-      <c r="B83" t="s">
-        <v>339</v>
-      </c>
-      <c r="C83">
-        <v>254</v>
-      </c>
-      <c r="D83" t="s">
-        <v>338</v>
+        <v>185</v>
       </c>
     </row>
     <row r="84" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A84" t="s">
-        <v>167</v>
+        <v>187</v>
+      </c>
+      <c r="B84" t="s">
+        <v>343</v>
+      </c>
+      <c r="C84">
+        <v>365</v>
+      </c>
+      <c r="D84" t="s">
+        <v>342</v>
       </c>
     </row>
     <row r="85" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A85" t="s">
-        <v>168</v>
+        <v>188</v>
       </c>
     </row>
     <row r="86" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A86" t="s">
-        <v>169</v>
+        <v>189</v>
       </c>
       <c r="B86" t="s">
-        <v>341</v>
+        <v>345</v>
       </c>
       <c r="C86">
-        <v>362</v>
+        <v>365</v>
       </c>
       <c r="D86" t="s">
-        <v>340</v>
+        <v>344</v>
       </c>
     </row>
     <row r="87" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A87" t="s">
-        <v>170</v>
+        <v>191</v>
       </c>
       <c r="B87" t="s">
-        <v>309</v>
+        <v>347</v>
       </c>
       <c r="C87">
-        <v>255</v>
+        <v>365</v>
       </c>
       <c r="D87" t="s">
-        <v>342</v>
+        <v>346</v>
       </c>
     </row>
     <row r="88" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A88" t="s">
-        <v>171</v>
+        <v>192</v>
       </c>
       <c r="B88" t="s">
-        <v>344</v>
+        <v>349</v>
       </c>
       <c r="C88">
-        <v>255</v>
+        <v>365</v>
       </c>
       <c r="D88" t="s">
-        <v>343</v>
+        <v>348</v>
       </c>
     </row>
     <row r="89" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A89" t="s">
-        <v>172</v>
+        <v>193</v>
+      </c>
+      <c r="B89" t="s">
+        <v>351</v>
+      </c>
+      <c r="C89">
+        <v>365</v>
+      </c>
+      <c r="D89" t="s">
+        <v>350</v>
       </c>
     </row>
     <row r="90" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A90" t="s">
-        <v>173</v>
+        <v>194</v>
       </c>
       <c r="B90" t="s">
-        <v>54</v>
+        <v>353</v>
       </c>
       <c r="C90">
         <v>365</v>
       </c>
       <c r="D90" t="s">
-        <v>345</v>
+        <v>352</v>
       </c>
     </row>
     <row r="91" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A91" t="s">
-        <v>174</v>
+        <v>197</v>
       </c>
       <c r="B91" t="s">
-        <v>347</v>
+        <v>355</v>
       </c>
       <c r="C91">
-        <v>254</v>
+        <v>365</v>
       </c>
       <c r="D91" t="s">
-        <v>346</v>
+        <v>354</v>
       </c>
     </row>
     <row r="92" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A92" t="s">
-        <v>175</v>
+        <v>198</v>
       </c>
       <c r="B92" t="s">
-        <v>349</v>
+        <v>357</v>
       </c>
       <c r="C92">
-        <v>260</v>
+        <v>365</v>
       </c>
       <c r="D92" t="s">
-        <v>348</v>
+        <v>356</v>
       </c>
     </row>
     <row r="93" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A93" t="s">
-        <v>247</v>
-      </c>
-      <c r="B93" t="s">
-        <v>351</v>
-      </c>
-      <c r="C93">
-        <v>366</v>
-      </c>
-      <c r="D93" t="s">
-        <v>350</v>
+        <v>199</v>
       </c>
     </row>
     <row r="94" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A94" t="s">
-        <v>185</v>
+        <v>200</v>
+      </c>
+      <c r="B94" t="s">
+        <v>359</v>
+      </c>
+      <c r="C94">
+        <v>365</v>
+      </c>
+      <c r="D94" t="s">
+        <v>358</v>
       </c>
     </row>
     <row r="95" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A95" t="s">
-        <v>187</v>
+        <v>202</v>
       </c>
       <c r="B95" t="s">
-        <v>353</v>
+        <v>361</v>
       </c>
       <c r="C95">
         <v>365</v>
       </c>
       <c r="D95" t="s">
-        <v>352</v>
+        <v>360</v>
       </c>
     </row>
     <row r="96" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A96" t="s">
-        <v>188</v>
+        <v>203</v>
+      </c>
+      <c r="D96" t="s">
+        <v>348</v>
       </c>
     </row>
     <row r="97" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A97" t="s">
-        <v>189</v>
+        <v>204</v>
       </c>
       <c r="B97" t="s">
-        <v>355</v>
+        <v>363</v>
       </c>
       <c r="C97">
         <v>365</v>
       </c>
       <c r="D97" t="s">
-        <v>354</v>
+        <v>362</v>
       </c>
     </row>
     <row r="98" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A98" t="s">
-        <v>191</v>
+        <v>205</v>
       </c>
       <c r="B98" t="s">
-        <v>357</v>
+        <v>365</v>
       </c>
       <c r="C98">
         <v>365</v>
       </c>
       <c r="D98" t="s">
-        <v>356</v>
+        <v>364</v>
       </c>
     </row>
     <row r="99" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A99" t="s">
-        <v>192</v>
-      </c>
-      <c r="B99" t="s">
-        <v>359</v>
-      </c>
-      <c r="C99">
-        <v>365</v>
+        <v>206</v>
       </c>
       <c r="D99" t="s">
-        <v>358</v>
+        <v>366</v>
       </c>
     </row>
     <row r="100" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A100" t="s">
-        <v>193</v>
-      </c>
-      <c r="B100" t="s">
-        <v>361</v>
-      </c>
-      <c r="C100">
-        <v>365</v>
-      </c>
-      <c r="D100" t="s">
-        <v>360</v>
+        <v>207</v>
       </c>
     </row>
     <row r="101" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A101" t="s">
-        <v>194</v>
+        <v>208</v>
       </c>
       <c r="B101" t="s">
-        <v>363</v>
+        <v>368</v>
       </c>
       <c r="C101">
         <v>365</v>
       </c>
       <c r="D101" t="s">
-        <v>362</v>
+        <v>367</v>
       </c>
     </row>
     <row r="102" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A102" t="s">
-        <v>197</v>
-      </c>
-      <c r="B102" t="s">
-        <v>365</v>
-      </c>
-      <c r="C102">
-        <v>365</v>
-      </c>
-      <c r="D102" t="s">
-        <v>364</v>
+        <v>210</v>
       </c>
     </row>
     <row r="103" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A103" t="s">
-        <v>198</v>
-      </c>
-      <c r="B103" t="s">
-        <v>367</v>
-      </c>
-      <c r="C103">
-        <v>365</v>
-      </c>
-      <c r="D103" t="s">
-        <v>366</v>
+        <v>213</v>
       </c>
     </row>
     <row r="104" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A104" t="s">
-        <v>199</v>
+        <v>214</v>
+      </c>
+      <c r="B104" t="s">
+        <v>370</v>
+      </c>
+      <c r="C104">
+        <v>266</v>
+      </c>
+      <c r="D104" t="s">
+        <v>369</v>
       </c>
     </row>
     <row r="105" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A105" t="s">
-        <v>200</v>
-      </c>
-      <c r="B105" t="s">
-        <v>369</v>
-      </c>
-      <c r="C105">
-        <v>365</v>
-      </c>
-      <c r="D105" t="s">
-        <v>368</v>
+        <v>215</v>
       </c>
     </row>
     <row r="106" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A106" t="s">
-        <v>202</v>
-      </c>
-      <c r="B106" t="s">
-        <v>371</v>
-      </c>
-      <c r="C106">
-        <v>365</v>
-      </c>
-      <c r="D106" t="s">
-        <v>370</v>
+        <v>217</v>
       </c>
     </row>
     <row r="107" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A107" t="s">
-        <v>203</v>
-      </c>
-      <c r="D107" t="s">
-        <v>358</v>
+        <v>218</v>
       </c>
     </row>
     <row r="108" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A108" t="s">
-        <v>204</v>
+        <v>219</v>
       </c>
       <c r="B108" t="s">
-        <v>373</v>
+        <v>372</v>
       </c>
       <c r="C108">
-        <v>365</v>
+        <v>261</v>
       </c>
       <c r="D108" t="s">
-        <v>372</v>
+        <v>371</v>
       </c>
     </row>
     <row r="109" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A109" t="s">
-        <v>205</v>
-      </c>
-      <c r="B109" t="s">
-        <v>375</v>
-      </c>
-      <c r="C109">
-        <v>365</v>
-      </c>
-      <c r="D109" t="s">
-        <v>374</v>
+        <v>221</v>
       </c>
     </row>
     <row r="110" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A110" t="s">
-        <v>206</v>
-      </c>
-      <c r="D110" t="s">
-        <v>376</v>
+        <v>222</v>
       </c>
     </row>
     <row r="111" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A111" t="s">
-        <v>207</v>
+        <v>223</v>
+      </c>
+      <c r="B111" t="s">
+        <v>374</v>
+      </c>
+      <c r="C111">
+        <v>258</v>
+      </c>
+      <c r="D111" t="s">
+        <v>373</v>
       </c>
     </row>
     <row r="112" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A112" t="s">
-        <v>208</v>
-      </c>
-      <c r="B112" t="s">
-        <v>378</v>
-      </c>
-      <c r="C112">
-        <v>365</v>
-      </c>
-      <c r="D112" t="s">
-        <v>377</v>
+        <v>224</v>
       </c>
     </row>
     <row r="113" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A113" t="s">
-        <v>210</v>
+        <v>225</v>
+      </c>
+      <c r="B113" t="s">
+        <v>376</v>
+      </c>
+      <c r="C113">
+        <v>266</v>
+      </c>
+      <c r="D113" t="s">
+        <v>375</v>
       </c>
     </row>
     <row r="114" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A114" t="s">
-        <v>213</v>
+        <v>226</v>
       </c>
     </row>
     <row r="115" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A115" t="s">
-        <v>214</v>
-      </c>
-      <c r="B115" t="s">
-        <v>380</v>
-      </c>
-      <c r="C115">
-        <v>266</v>
-      </c>
-      <c r="D115" t="s">
-        <v>379</v>
+        <v>227</v>
       </c>
     </row>
     <row r="116" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A116" t="s">
-        <v>215</v>
+        <v>228</v>
       </c>
     </row>
     <row r="117" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A117" t="s">
-        <v>217</v>
+        <v>229</v>
+      </c>
+      <c r="B117" t="s">
+        <v>378</v>
+      </c>
+      <c r="C117">
+        <v>362</v>
+      </c>
+      <c r="D117" t="s">
+        <v>377</v>
       </c>
     </row>
     <row r="118" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A118" t="s">
-        <v>218</v>
+        <v>231</v>
       </c>
     </row>
     <row r="119" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A119" t="s">
-        <v>219</v>
-      </c>
-      <c r="B119" t="s">
-        <v>382</v>
-      </c>
-      <c r="C119">
-        <v>261</v>
-      </c>
-      <c r="D119" t="s">
-        <v>381</v>
+        <v>232</v>
       </c>
     </row>
     <row r="120" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A120" t="s">
-        <v>221</v>
+        <v>234</v>
       </c>
     </row>
     <row r="121" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A121" t="s">
-        <v>222</v>
+        <v>235</v>
       </c>
     </row>
     <row r="122" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A122" t="s">
-        <v>223</v>
-      </c>
-      <c r="B122" t="s">
-        <v>384</v>
-      </c>
-      <c r="C122">
-        <v>258</v>
-      </c>
-      <c r="D122" t="s">
-        <v>383</v>
+        <v>236</v>
       </c>
     </row>
     <row r="123" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A123" t="s">
-        <v>224</v>
+        <v>238</v>
+      </c>
+      <c r="B123" t="s">
+        <v>380</v>
+      </c>
+      <c r="C123">
+        <v>266</v>
+      </c>
+      <c r="D123" t="s">
+        <v>379</v>
       </c>
     </row>
     <row r="124" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A124" t="s">
-        <v>225</v>
+        <v>239</v>
       </c>
       <c r="B124" t="s">
-        <v>386</v>
+        <v>382</v>
       </c>
       <c r="C124">
         <v>266</v>
       </c>
       <c r="D124" t="s">
-        <v>385</v>
-      </c>
-    </row>
-    <row r="125" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A125" t="s">
-        <v>226</v>
-      </c>
-    </row>
-    <row r="126" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A126" t="s">
-        <v>227</v>
-      </c>
-    </row>
-    <row r="127" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A127" t="s">
-        <v>228</v>
-      </c>
-    </row>
-    <row r="128" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A128" t="s">
-        <v>229</v>
-      </c>
-      <c r="B128" t="s">
-        <v>388</v>
-      </c>
-      <c r="C128">
-        <v>362</v>
-      </c>
-      <c r="D128" t="s">
-        <v>387</v>
-      </c>
-    </row>
-    <row r="129" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A129" t="s">
-        <v>231</v>
-      </c>
-    </row>
-    <row r="130" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A130" t="s">
-        <v>232</v>
-      </c>
-    </row>
-    <row r="131" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A131" t="s">
-        <v>234</v>
-      </c>
-    </row>
-    <row r="132" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A132" t="s">
-        <v>235</v>
-      </c>
-    </row>
-    <row r="133" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A133" t="s">
-        <v>236</v>
-      </c>
-    </row>
-    <row r="134" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A134" t="s">
-        <v>238</v>
-      </c>
-      <c r="B134" t="s">
-        <v>390</v>
-      </c>
-      <c r="C134">
-        <v>266</v>
-      </c>
-      <c r="D134" t="s">
-        <v>389</v>
-      </c>
-    </row>
-    <row r="135" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A135" t="s">
-        <v>239</v>
-      </c>
-      <c r="B135" t="s">
-        <v>392</v>
-      </c>
-      <c r="C135">
-        <v>266</v>
-      </c>
-      <c r="D135" t="s">
-        <v>391</v>
+        <v>381</v>
       </c>
     </row>
   </sheetData>

</xml_diff>